<commit_message>
footer pushed and adde mode changes to excel
</commit_message>
<xml_diff>
--- a/Workings.xlsx
+++ b/Workings.xlsx
@@ -5,26 +5,27 @@
   <fileSharing readOnlyRecommended="0" userName="Office"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView activeTab="2" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Homepage" sheetId="1" r:id="rId4"/>
-    <sheet name="Vendor Panel" sheetId="2" r:id="rId5"/>
+    <sheet name="Homepage - Functioning" sheetId="1" r:id="rId4"/>
+    <sheet name="Vendor Panel - Functioning" sheetId="2" r:id="rId5"/>
+    <sheet name="Client Page Wise List" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1752338804" val="1224" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1752338804" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1752338804" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1752338804"/>
+      <pm:revision xmlns:pm="smNativeData" day="1752491624" val="1224" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1752491624" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1752491624" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1752491624"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="233">
   <si>
     <t>Logo</t>
   </si>
@@ -260,6 +261,15 @@
     <t>Link with related page</t>
   </si>
   <si>
+    <t>Footer</t>
+  </si>
+  <si>
+    <t>Our Industries Full Spacing and Alignment</t>
+  </si>
+  <si>
+    <t>Spacing</t>
+  </si>
+  <si>
     <t>Analytics</t>
   </si>
   <si>
@@ -426,13 +436,301 @@
   </si>
   <si>
     <t>Edit Shop Info</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Home Page</t>
+  </si>
+  <si>
+    <t>Reduce the Frame size apx 5mm to fit in 14'inch monitor</t>
+  </si>
+  <si>
+    <t>Red Banner is slider image about webstie offers. Slide 5-6 banners</t>
+  </si>
+  <si>
+    <t>Footer need to modify as per suggested design check wthsap</t>
+  </si>
+  <si>
+    <t>Shortcut of featues is not linkedin on related pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 Banner for 7 features in center and solution banner need to correct write S in logo and keep 3 design banner of each solution </t>
+  </si>
+  <si>
+    <t>Stock Sell</t>
+  </si>
+  <si>
+    <t>Neeed to correct pic size, strict size to uplaod the pic as its strecthing. Inquire button need to adjust below the address</t>
+  </si>
+  <si>
+    <t>apply effect, keep the center frame of product list as per figma</t>
+  </si>
+  <si>
+    <t>Countries in sorting pannel is messing</t>
+  </si>
+  <si>
+    <t>Contry flat is not there in the prodcut result in the center . Where country is mentioned pls put flag</t>
+  </si>
+  <si>
+    <t>Reset button as discussed , need to develop on sorting pannel on the top or below in the left corner or on top at right corner</t>
+  </si>
+  <si>
+    <t>Buy lead</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I sent one RFq but its not showing as discussed. It will reflect after one hr. also its not showing in the admin or vendor</t>
+  </si>
+  <si>
+    <t>also not showing on the home page</t>
+  </si>
+  <si>
+    <t>Current ticket desgin is not going well. Need improvement. Fonts are looking bigger and frame is mall. Discuss with pawan sir</t>
+  </si>
+  <si>
+    <t>and update accordingly</t>
+  </si>
+  <si>
+    <t>on product profile page, address of vendor - keep that frame and give red shadow and change color white instead of red shade</t>
+  </si>
+  <si>
+    <t>All inquire now- should be received in admin as notification, vendor as chat in marketplace and inbox and notifification on home</t>
+  </si>
+  <si>
+    <t>Sell offer</t>
+  </si>
+  <si>
+    <t>Need to design it properly. Discuss with pawan sir and design in best possible way. Heading size fonts must match with other pages</t>
+  </si>
+  <si>
+    <t>Check all inquiry is going in admin as notification, vendor as chat, notification on home page</t>
+  </si>
+  <si>
+    <t>Just add inquiry button and open inquiry box same as displaying in inquiry button on marketplace</t>
+  </si>
+  <si>
+    <t>Check the sent inquiry is coming in the admin dashbaord or not</t>
+  </si>
+  <si>
+    <t>vendor or buyer will get a notification that inquiry has been sent and team will contact you shortly</t>
+  </si>
+  <si>
+    <t>Design I AM HIRING page - put dummy details from vendor dashbaord</t>
+  </si>
+  <si>
+    <t>Job seekers page- adjust it as per figma design accuratly . Upload and check job seeker form and apply job and check effect in</t>
+  </si>
+  <si>
+    <t>vendor dahbaord and admin dashbaord</t>
+  </si>
+  <si>
+    <t>all notification of job upload and job applied and job seeker profile updlaod should goes into Industry jobs tab on admin pannel</t>
+  </si>
+  <si>
+    <t>Trade shows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wokring but check the flow and forms and upload data from admin dashboard if working properly then good close it </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Working fine</t>
+  </si>
+  <si>
+    <t>Supplier icon</t>
+  </si>
+  <si>
+    <t>but log in as supplier and showing already loin in buyer and hire icon also, that should be restrict supplier cant see buyer log in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">as already log in </t>
+  </si>
+  <si>
+    <t>Buyer icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Same as above</t>
+  </si>
+  <si>
+    <t>Hire icon</t>
+  </si>
+  <si>
+    <t>Wokring fine</t>
+  </si>
+  <si>
+    <t>Feature icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  All feature should be linkedin on the related pages</t>
+  </si>
+  <si>
+    <t>Design the page more attaractivly</t>
+  </si>
+  <si>
+    <t>Translate icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add more languages </t>
+  </si>
+  <si>
+    <t>All categories tab</t>
+  </si>
+  <si>
+    <t>Try and check - remove the border</t>
+  </si>
+  <si>
+    <t>Admin DB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List down what are the result you are showing and how you are presenting. I need the list first to make it better, then start the develeopment </t>
+  </si>
+  <si>
+    <t>Product approval</t>
+  </si>
+  <si>
+    <t>Check the previousely suggested changes in the form. If that has done then mark it 100%</t>
+  </si>
+  <si>
+    <t>product approvel should go in the admin Db. Check and mark</t>
+  </si>
+  <si>
+    <t>in Db it fresh request should show on the top with date when vendor uploaded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendor approval </t>
+  </si>
+  <si>
+    <t>Show recent req on the top of the list and with date when he requested</t>
+  </si>
+  <si>
+    <t>currently its not working as I created one vendor at 12 pm and now 6.30 its not showing in the approval list in vendor</t>
+  </si>
+  <si>
+    <t>LEAD</t>
+  </si>
+  <si>
+    <t>Lead means all leads or only RFQ. Define it or msg on whatsap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sorting pannel is messy. Discuss with pawan sir and design it properly. </t>
+  </si>
+  <si>
+    <t>Reduce the space from the top above sortin bar</t>
+  </si>
+  <si>
+    <t>show recent sell offer listing on the top. Sell offer notification should go into the admin inbox also when supplier upload and</t>
+  </si>
+  <si>
+    <t>buyer click on inquire</t>
+  </si>
+  <si>
+    <t>Stock sell</t>
+  </si>
+  <si>
+    <t>You should discuss with pawan sir and redisgn the inteface when opening any tab/feature. All are messed look wise . Coding and</t>
+  </si>
+  <si>
+    <t xml:space="preserve">functioning is good but look is messed up completely </t>
+  </si>
+  <si>
+    <t>Trade show</t>
+  </si>
+  <si>
+    <t>Manage trade show tab - when click showing code page</t>
+  </si>
+  <si>
+    <t>As you have already shown Leads above then this buy lead can removed. Lead means that feature will have all leads received</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from RFQ-MARETPLACE-SELL OFFER- STOCK SELL and admin can see the list and download according to the feature. If wants to </t>
+  </si>
+  <si>
+    <t>Buyer</t>
+  </si>
+  <si>
+    <t>Design the interface</t>
+  </si>
+  <si>
+    <t>Show recent reg buyer and for approal first</t>
+  </si>
+  <si>
+    <t>Mention date when he registered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guest </t>
+  </si>
+  <si>
+    <t>Guest account is buyer. U can remove this tab</t>
+  </si>
+  <si>
+    <t>Industry jobs</t>
+  </si>
+  <si>
+    <t>Re design interface sorting - results - check all and make it 100%</t>
+  </si>
+  <si>
+    <t>Graphic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make it workigng - check all flow and result . Should work smoothly. </t>
+  </si>
+  <si>
+    <t>Deal assist</t>
+  </si>
+  <si>
+    <t>Place button on the deal assit homepage and that inquiry shold come here and in inbox of admin under Deal assist same like</t>
+  </si>
+  <si>
+    <t>stock sell inquiry comes in the inbox</t>
+  </si>
+  <si>
+    <t>On going</t>
+  </si>
+  <si>
+    <t>Redesgin the interface and test and make it 100% active with all type of membership</t>
+  </si>
+  <si>
+    <t>Home page</t>
+  </si>
+  <si>
+    <t>Homepage uplaod if you are mentioning here. Or you can keep in the graphic as home page graphic as there is no other featuer</t>
+  </si>
+  <si>
+    <t>on the home page so you can remove from here and keep it in the graphic tab only</t>
+  </si>
+  <si>
+    <t>Workign fine</t>
+  </si>
+  <si>
+    <t>Update as we discussed</t>
+  </si>
+  <si>
+    <t>Fin &amp; account</t>
+  </si>
+  <si>
+    <t>We will design it in the last. Plan to show no of vendor -paid memebr- type- region- collection- when is going to end. Format to</t>
+  </si>
+  <si>
+    <t>issue invoice, download all invoices as per date month year wise. Tax calculatjion if any, manage working expecences list heading</t>
+  </si>
+  <si>
+    <t>Dashboard allotment</t>
+  </si>
+  <si>
+    <t>Will test and finalise the flow and working</t>
+  </si>
+  <si>
+    <t>Gravience n complain</t>
+  </si>
+  <si>
+    <t>inbox type where all request will receive from homepage (Grav*comp)if any user click and file grav or complain. Admin will</t>
+  </si>
+  <si>
+    <t xml:space="preserve">receive this in grav n complain inbox and it will also display in admin notifistion on dashabord </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="5" formatCode="#,##0\ &quot;$&quot;;\-#,##0\ &quot;$&quot;"/>
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;$&quot;;[Red]\-#,##0\ &quot;$&quot;"/>
     <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;$&quot;;\-#,##0.00\ &quot;$&quot;"/>
@@ -441,6 +739,7 @@
     <numFmt numFmtId="41" formatCode="_-* #,##0\ _$_-;\-* #,##0\ _$_-;_-* &quot;-&quot;\ _$_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
+    <numFmt numFmtId="9" formatCode="0%"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -450,7 +749,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1752338804" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1752491624" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -466,7 +765,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1752338804" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1752491624" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -481,7 +780,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1752338804" fgClr="007F00" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1752491624" fgClr="007F00" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -496,7 +795,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1752338804" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1752491624" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="160" lang="default"/>
             <pm:ea face="SimSun" sz="160" lang="default"/>
@@ -512,7 +811,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1752338804" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1752491624" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="160" lang="default"/>
             <pm:ea face="SimSun" sz="160" lang="default"/>
@@ -527,7 +826,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1752338804" fgClr="007F00" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1752491624" fgClr="007F00" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="160" lang="default"/>
             <pm:ea face="SimSun" sz="160" lang="default"/>
@@ -536,7 +835,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -549,19 +848,8 @@
     <fill>
       <patternFill patternType="none"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1752338804" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -577,7 +865,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1752338804"/>
+          <pm:border xmlns:pm="smNativeData" id="1752491624"/>
         </ext>
       </extLst>
     </border>
@@ -596,7 +884,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1752338804">
+          <pm:border xmlns:pm="smNativeData" id="1752491624">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -620,7 +908,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1752338804">
+          <pm:border xmlns:pm="smNativeData" id="1752491624">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -628,30 +916,11 @@
         </ext>
       </extLst>
     </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1752338804"/>
-        </ext>
-      </extLst>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -671,6 +940,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -678,7 +949,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1752338804" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1752491624" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
     </ext>
@@ -942,10 +1213,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView view="normal" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.75"/>
@@ -1359,12 +1630,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:3">
       <c r="A66"/>
       <c r="C66" t="s">
         <v>63</v>
       </c>
-      <c r="E66"/>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="8" t="s">
@@ -1427,13 +1697,32 @@
       </c>
       <c r="C80" s="7" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="3:5">
+      <c r="C83" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1752338804" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1752491624" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1442,16 +1731,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1752338804" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1752338804" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752338804" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752338804" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1752491624" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1752491624" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752491624" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752491624" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752338804" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752491624" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1464,8 +1753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView view="normal" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.75"/>
@@ -1477,16 +1766,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E1" s="10"/>
     </row>
     <row r="2" spans="3:3">
       <c r="C2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1495,15 +1784,15 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="3:5">
       <c r="C5" s="5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>4</v>
@@ -1511,7 +1800,7 @@
     </row>
     <row r="6" spans="3:5">
       <c r="C6" s="5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>4</v>
@@ -1519,7 +1808,7 @@
     </row>
     <row r="7" spans="3:5">
       <c r="C7" s="5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>4</v>
@@ -1527,10 +1816,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>4</v>
@@ -1538,7 +1827,7 @@
     </row>
     <row r="10" spans="3:5">
       <c r="C10" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>4</v>
@@ -1546,7 +1835,7 @@
     </row>
     <row r="11" spans="3:5">
       <c r="C11" s="5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>4</v>
@@ -1554,7 +1843,7 @@
     </row>
     <row r="12" spans="3:5">
       <c r="C12" s="5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>4</v>
@@ -1562,7 +1851,7 @@
     </row>
     <row r="13" spans="3:5">
       <c r="C13" s="5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>4</v>
@@ -1570,36 +1859,36 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="3:3">
       <c r="C16" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="3:3">
       <c r="C17" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>4</v>
@@ -1607,22 +1896,22 @@
     </row>
     <row r="22" spans="3:3">
       <c r="C22" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="3:3">
       <c r="C23" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="3:3">
       <c r="C24" s="5" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="3:5">
       <c r="C25" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>4</v>
@@ -1630,10 +1919,10 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>4</v>
@@ -1641,10 +1930,10 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>4</v>
@@ -1652,17 +1941,17 @@
     </row>
     <row r="30" spans="3:3">
       <c r="C30" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="3:3">
       <c r="C31" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="3:5">
       <c r="C32" s="5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>4</v>
@@ -1670,7 +1959,7 @@
     </row>
     <row r="33" spans="3:5">
       <c r="C33" s="5" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>4</v>
@@ -1678,23 +1967,23 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C35" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="3:3">
       <c r="C36" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>4</v>
@@ -1702,7 +1991,7 @@
     </row>
     <row r="39" spans="3:5">
       <c r="C39" s="5" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>4</v>
@@ -1710,12 +1999,12 @@
     </row>
     <row r="40" spans="3:3">
       <c r="C40" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="3:5">
       <c r="C41" s="5" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>4</v>
@@ -1723,28 +2012,28 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C43" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="3:3">
       <c r="C44" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="3:3">
       <c r="C45" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>4</v>
@@ -1752,18 +2041,18 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C49" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>4</v>
@@ -1771,10 +2060,10 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>4</v>
@@ -1782,17 +2071,17 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C55" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1752338804" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1752491624" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1801,16 +2090,648 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1752338804" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1752338804" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752338804" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752338804" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1752491624" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1752491624" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752491624" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752491624" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752338804" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752491624" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <dimension ref="A1:E109"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
+  <cols>
+    <col min="1" max="1" width="14.621622" customWidth="1"/>
+    <col min="3" max="3" width="112.531532" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="11" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="2" spans="3:3">
+      <c r="C2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3">
+      <c r="C3" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3">
+      <c r="C4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3">
+      <c r="C5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" s="11" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3">
+      <c r="C8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="3:3">
+      <c r="C9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="3:3">
+      <c r="C10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="3:3">
+      <c r="C11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13" t="s">
+        <v>150</v>
+      </c>
+      <c r="E13" s="11" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="14" spans="3:3">
+      <c r="C14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" s="11" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" t="s">
+        <v>157</v>
+      </c>
+      <c r="E21" s="11" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3">
+      <c r="C22" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" t="s">
+        <v>159</v>
+      </c>
+      <c r="E24" s="11" t="n">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3">
+      <c r="C25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3">
+      <c r="C26" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" t="s">
+        <v>162</v>
+      </c>
+      <c r="E28" s="11" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3">
+      <c r="C29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3">
+      <c r="C30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3">
+      <c r="C31" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>166</v>
+      </c>
+      <c r="C33" t="s">
+        <v>167</v>
+      </c>
+      <c r="E33" s="11" t="n">
+        <v>0.980000000000000071</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>168</v>
+      </c>
+      <c r="E35" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>169</v>
+      </c>
+      <c r="C37" t="s">
+        <v>168</v>
+      </c>
+      <c r="E37" s="11" t="n">
+        <v>0.980000000000000071</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>172</v>
+      </c>
+      <c r="C41" t="s">
+        <v>173</v>
+      </c>
+      <c r="E41" s="11" t="n">
+        <v>0.980000000000000071</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>174</v>
+      </c>
+      <c r="C43" t="s">
+        <v>173</v>
+      </c>
+      <c r="E43" s="11" t="n">
+        <v>0.980000000000000071</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" t="s">
+        <v>175</v>
+      </c>
+      <c r="E45" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>176</v>
+      </c>
+      <c r="C47" t="s">
+        <v>177</v>
+      </c>
+      <c r="E47" s="11" t="n">
+        <v>0.980000000000000071</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3">
+      <c r="C48" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>179</v>
+      </c>
+      <c r="C50" t="s">
+        <v>180</v>
+      </c>
+      <c r="E50" s="11" t="n">
+        <v>0.980000000000000071</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>181</v>
+      </c>
+      <c r="C52" t="s">
+        <v>182</v>
+      </c>
+      <c r="E52" s="11" t="n">
+        <v>0.990000000000000036</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>81</v>
+      </c>
+      <c r="C55" t="s">
+        <v>184</v>
+      </c>
+      <c r="E55" s="11" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>185</v>
+      </c>
+      <c r="C57" t="s">
+        <v>186</v>
+      </c>
+      <c r="E57" s="11" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3">
+      <c r="C58" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3">
+      <c r="C59" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>189</v>
+      </c>
+      <c r="C61" t="s">
+        <v>190</v>
+      </c>
+      <c r="E61" s="11" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3">
+      <c r="C62" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>192</v>
+      </c>
+      <c r="C64" t="s">
+        <v>193</v>
+      </c>
+      <c r="E64" s="11" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3">
+      <c r="C65" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>156</v>
+      </c>
+      <c r="C67" t="s">
+        <v>195</v>
+      </c>
+      <c r="E67" s="11" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3">
+      <c r="C68" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3">
+      <c r="C69" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>198</v>
+      </c>
+      <c r="C71" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3">
+      <c r="C72" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>201</v>
+      </c>
+      <c r="C74" t="s">
+        <v>202</v>
+      </c>
+      <c r="E74" s="11" t="n">
+        <v>0.980000000000000071</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>149</v>
+      </c>
+      <c r="C76" t="s">
+        <v>203</v>
+      </c>
+      <c r="E76" s="11" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3">
+      <c r="C77" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>205</v>
+      </c>
+      <c r="C79" t="s">
+        <v>206</v>
+      </c>
+      <c r="E79" s="11" t="n">
+        <v>0.980000000000000071</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3">
+      <c r="C80" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3">
+      <c r="C81" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="11"/>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="C83" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="11"/>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="C85" t="s">
+        <v>212</v>
+      </c>
+      <c r="E85" s="11" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="11"/>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>213</v>
+      </c>
+      <c r="C87" t="s">
+        <v>214</v>
+      </c>
+      <c r="E87" s="11" t="n">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>215</v>
+      </c>
+      <c r="C89" t="s">
+        <v>216</v>
+      </c>
+      <c r="E89" s="11" t="n">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="90" spans="3:3">
+      <c r="C90" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>84</v>
+      </c>
+      <c r="C92" t="s">
+        <v>218</v>
+      </c>
+      <c r="E92" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>129</v>
+      </c>
+      <c r="C94" t="s">
+        <v>219</v>
+      </c>
+      <c r="E94" s="11" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>220</v>
+      </c>
+      <c r="C96" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3">
+      <c r="C97" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>133</v>
+      </c>
+      <c r="C99" t="s">
+        <v>223</v>
+      </c>
+      <c r="E99" s="11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>78</v>
+      </c>
+      <c r="C101" t="s">
+        <v>224</v>
+      </c>
+      <c r="E101" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" t="s">
+        <v>225</v>
+      </c>
+      <c r="C103" t="s">
+        <v>226</v>
+      </c>
+      <c r="E103" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="3:3">
+      <c r="C104" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" t="s">
+        <v>228</v>
+      </c>
+      <c r="C106" t="s">
+        <v>229</v>
+      </c>
+      <c r="E106" s="11" t="n">
+        <v>0.980000000000000071</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" t="s">
+        <v>230</v>
+      </c>
+      <c r="C108" t="s">
+        <v>231</v>
+      </c>
+      <c r="E108" s="11" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="109" spans="3:3">
+      <c r="C109" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1752491624" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="1.000000" right="1.000000" top="1.000000" bottom="1.000000" header="0.393750" footer="0.393750"/>
+  <pageSetup paperSize="1" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1752491624" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1752491624" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752491624" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752491624" Id="1" type="0" value="0"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752491624" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Speed Up Email Sending Needs to be Tested
</commit_message>
<xml_diff>
--- a/Workings.xlsx
+++ b/Workings.xlsx
@@ -16,10 +16,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1752596489" val="1224" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1752596489" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1752596489" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1752596489"/>
+      <pm:revision xmlns:pm="smNativeData" day="1752735554" val="1224" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1752735554" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1752735554" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1752735554"/>
     </ext>
   </extLst>
 </workbook>
@@ -756,7 +756,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1752596489" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1752735554" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -771,7 +771,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1752596489" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1752735554" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -786,7 +786,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1752596489" fgClr="007F00" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1752735554" fgClr="007F00" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -802,7 +802,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1752596489" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1752735554" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="200" lang="default" weight="bold"/>
@@ -817,7 +817,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1752596489" fgClr="007F00" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1752735554" fgClr="007F00" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -833,7 +833,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1752596489" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1752735554" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -842,7 +842,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -852,8 +852,19 @@
     <fill>
       <patternFill patternType="none"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1752735554" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -869,7 +880,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1752596489"/>
+          <pm:border xmlns:pm="smNativeData" id="1752735554"/>
         </ext>
       </extLst>
     </border>
@@ -888,12 +899,31 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1752596489">
+          <pm:border xmlns:pm="smNativeData" id="1752735554">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1752735554"/>
         </ext>
       </extLst>
     </border>
@@ -938,7 +968,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1752596489" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1752735554" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -1739,7 +1769,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1752596489" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1752735554" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1748,16 +1778,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1752596489" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1752596489" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752596489" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752596489" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1752735554" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1752735554" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752735554" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752735554" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752596489" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752735554" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2119,7 +2149,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1752596489" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1752735554" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2128,16 +2158,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1752596489" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1752596489" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752596489" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752596489" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1752735554" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1752735554" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752735554" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752735554" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752596489" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752735554" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2153,8 +2183,8 @@
   </sheetPr>
   <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -2356,7 +2386,7 @@
       <c r="A35" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="9" t="s">
         <v>168</v>
       </c>
       <c r="E35" s="1" t="n">
@@ -2492,12 +2522,12 @@
       </c>
     </row>
     <row r="58" spans="3:3" ht="18.75" customHeight="1">
-      <c r="C58" t="s">
+      <c r="C58" s="12" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="59" spans="3:3" ht="18.75" customHeight="1">
-      <c r="C59" t="s">
+      <c r="C59" s="12" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2790,7 +2820,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1752596489" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1752735554" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2799,16 +2829,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1752596489" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1752596489" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752596489" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752596489" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1752735554" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1752735554" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752735554" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752735554" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752596489" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752735554" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2848,7 +2878,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1752596489" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1752735554" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2857,16 +2887,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1752596489" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1752596489" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752596489" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752596489" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1752735554" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1752735554" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752735554" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752735554" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752596489" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752735554" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Added Banners and Minor Fixes
</commit_message>
<xml_diff>
--- a/Workings.xlsx
+++ b/Workings.xlsx
@@ -16,10 +16,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1752735554" val="1224" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1752735554" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1752735554" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1752735554"/>
+      <pm:revision xmlns:pm="smNativeData" day="1752739665" val="1224" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1752739665" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1752739665" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1752739665"/>
     </ext>
   </extLst>
 </workbook>
@@ -756,7 +756,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1752735554" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1752739665" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -771,7 +771,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1752735554" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1752739665" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -786,7 +786,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1752735554" fgClr="007F00" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1752739665" fgClr="007F00" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -802,7 +802,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1752735554" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1752739665" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="200" lang="default" weight="bold"/>
@@ -817,7 +817,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1752735554" fgClr="007F00" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1752739665" fgClr="007F00" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -833,7 +833,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1752735554" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1752739665" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -858,7 +858,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1752735554" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1752739665" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -880,7 +880,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1752735554"/>
+          <pm:border xmlns:pm="smNativeData" id="1752739665"/>
         </ext>
       </extLst>
     </border>
@@ -899,7 +899,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1752735554">
+          <pm:border xmlns:pm="smNativeData" id="1752739665">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -923,7 +923,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1752735554"/>
+          <pm:border xmlns:pm="smNativeData" id="1752739665"/>
         </ext>
       </extLst>
     </border>
@@ -931,7 +931,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -960,7 +960,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -968,7 +967,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1752735554" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1752739665" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -1769,7 +1768,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1752735554" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1752739665" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1778,16 +1777,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1752735554" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1752735554" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752735554" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752735554" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1752739665" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1752739665" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752739665" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752739665" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752735554" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752739665" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2149,7 +2148,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1752735554" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1752739665" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2158,16 +2157,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1752735554" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1752735554" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752735554" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752735554" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1752739665" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1752739665" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752739665" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752739665" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752735554" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752739665" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2183,8 +2182,8 @@
   </sheetPr>
   <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -2522,12 +2521,12 @@
       </c>
     </row>
     <row r="58" spans="3:3" ht="18.75" customHeight="1">
-      <c r="C58" s="12" t="s">
+      <c r="C58" s="9" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="59" spans="3:3" ht="18.75" customHeight="1">
-      <c r="C59" s="12" t="s">
+      <c r="C59" s="9" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2820,7 +2819,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1752735554" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1752739665" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2829,16 +2828,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1752735554" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1752735554" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752735554" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752735554" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1752739665" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1752739665" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752739665" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752739665" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752735554" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752739665" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2878,7 +2877,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1752735554" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1752739665" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2887,16 +2886,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1752735554" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1752735554" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752735554" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1752735554" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1752739665" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1752739665" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752739665" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1752739665" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752735554" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1752739665" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>